<commit_message>
Remarques prises en compte
</commit_message>
<xml_diff>
--- a/rapport/Hennion-Nourrisson.xlsx
+++ b/rapport/Hennion-Nourrisson.xlsx
@@ -93,7 +93,7 @@
     <t xml:space="preserve">Au vu de votre jeu, il semble qu'il doit y avoir d'autres textures, pour représenter les armes par exemple.</t>
   </si>
   <si>
-    <t xml:space="preserve">Les textures d’armes n’étaient pas encore trouvées, elles ont été ajoutées par la suite</t>
+    <t xml:space="preserve">Les textures d’armes n’étaient pas encore trouvées, elles ont été ajoutées par la suite. Si jamais nous trouvons d’autres textures comme des décors supplémentaires nous les ajouterons, mais pour l’instant rien n’a été rajouté.</t>
   </si>
   <si>
     <t xml:space="preserve">Non</t>
@@ -303,15 +303,15 @@
   <dimension ref="A2:D29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.9554655870445"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.3846153846154"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="60.5222672064777"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.0566801619433"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -435,7 +435,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
         <v>2</v>
       </c>

</xml_diff>